<commit_message>
Added the Solution files
</commit_message>
<xml_diff>
--- a/Investments.xlsx
+++ b/Investments.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chiranjeev\Documents\Investment case study Cohort-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Case study Spark funds\Case_study_submission\Case_study_submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9087DB07-4B95-4976-A827-AF638FC2C244}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table -1.1" sheetId="2" r:id="rId1"/>
@@ -17,11 +18,8 @@
     <sheet name="Table-3.1" sheetId="5" r:id="rId3"/>
     <sheet name="Table-5.1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>C1</t>
   </si>
@@ -357,12 +355,76 @@
   </si>
   <si>
     <t>Sector-wise Investment Analysis</t>
+  </si>
+  <si>
+    <t>permalink</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>114949 rows × 16 columns</t>
+  </si>
+  <si>
+    <t>venture</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>Social,Finance,Analytics,Advertising</t>
+  </si>
+  <si>
+    <t>Cleantech/Semiconductors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107766584223.0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5379078691.0
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News, Search and Messaging
+</t>
+  </si>
+  <si>
+    <t>DueDil</t>
+  </si>
+  <si>
+    <t>ARPU</t>
+  </si>
+  <si>
+    <t>Ameyo</t>
+  </si>
+  <si>
+    <t>Bacula Systems</t>
+  </si>
+  <si>
+    <t>17zuoye</t>
+  </si>
+  <si>
+    <t>Akosha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -569,11 +631,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -632,48 +707,59 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,7 +820,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -786,7 +872,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -987,38 +1073,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="3"/>
-    <col min="2" max="2" width="63.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1038,7 +1124,9 @@
       <c r="B5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17">
+        <v>66370</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1047,7 +1135,9 @@
       <c r="B6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17">
+        <v>66368</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1056,7 +1146,9 @@
       <c r="B7" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1065,7 +1157,9 @@
       <c r="B8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1074,7 +1168,9 @@
       <c r="B9" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11"/>
@@ -1098,40 +1194,41 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -1151,7 +1248,9 @@
       <c r="B5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="25">
+        <v>11748950</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
@@ -1160,7 +1259,9 @@
       <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="25">
+        <v>958694.5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
@@ -1169,7 +1270,9 @@
       <c r="B7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="12"/>
+      <c r="C7" s="25">
+        <v>719818</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1178,7 +1281,9 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="25">
+        <v>73308590</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
@@ -1187,7 +1292,9 @@
       <c r="B9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1210,11 +1317,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,21 +1332,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1259,7 +1366,9 @@
       <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1268,7 +1377,9 @@
       <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1277,7 +1388,9 @@
       <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1299,167 +1412,232 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
     <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="30"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="B1" s="33"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="24" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>1</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="26">
+        <v>12064</v>
+      </c>
+      <c r="D5" s="17">
+        <v>621</v>
+      </c>
+      <c r="E5" s="17">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="19">
         <v>2</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="38">
+        <v>2949543602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
         <v>3</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>4</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="42"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>5</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="41"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="19">
         <v>6</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="17">
+        <v>2950</v>
+      </c>
+      <c r="D10" s="17">
+        <v>147</v>
+      </c>
+      <c r="E10" s="17">
+        <v>110</v>
+      </c>
+      <c r="F10" s="42"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="19">
         <v>7</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="17">
+        <v>2714</v>
+      </c>
+      <c r="D11" s="17">
+        <v>133</v>
+      </c>
+      <c r="E11" s="17">
+        <v>60</v>
+      </c>
+      <c r="F11" s="41"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="19">
         <v>8</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C12" s="17">
+        <v>2350</v>
+      </c>
+      <c r="D12" s="17">
+        <v>130</v>
+      </c>
+      <c r="E12" s="17">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="19">
         <v>9</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>10</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1486,7 +1664,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E14">
+  <conditionalFormatting sqref="A5:E12 F7 F9 F11 A14:E14 A13:B13 D13:E13">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>